<commit_message>
added employee creation testcase
</commit_message>
<xml_diff>
--- a/TestData/OrangeHRMData.xlsx
+++ b/TestData/OrangeHRMData.xlsx
@@ -1,14 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA5CB51-3252-46DC-A638-FD1949EA0D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="User" sheetId="2" r:id="rId2"/>
+    <sheet name="EmpData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>EmpName</t>
   </si>
@@ -53,12 +55,33 @@
   </si>
   <si>
     <t>Sai_502</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>Test3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -406,20 +429,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -427,7 +450,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -442,21 +465,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -470,7 +493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -486,9 +509,69 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE2C4F3C-DE5B-4D0D-829E-06F08E95C9F2}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>